<commit_message>
Modified STEP files for complete 3D representation of the board
</commit_message>
<xml_diff>
--- a/pIRfusiX_sensorBoard/Project Outputs for pIRfusiX_sensorBoard/pIRfusiX_sensorBoard_BOM.xlsx
+++ b/pIRfusiX_sensorBoard/Project Outputs for pIRfusiX_sensorBoard/pIRfusiX_sensorBoard_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\randy\Documents\GitHub\SensorBoard\pIRfusiX_sensorBoard\Project Outputs for pIRfusiX_sensorBoard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RJ/Desktop/SensorBoard/pIRfusiX_sensorBoard/Project Outputs for pIRfusiX_sensorBoard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D9F9CB-417B-458B-8392-1F121217859A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED45096-2883-4046-8471-45D523934E95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2328" yWindow="312" windowWidth="17280" windowHeight="8964" xr2:uid="{7EA8B866-5E4B-4CBD-B814-F254738EF465}"/>
+    <workbookView xWindow="-20360" yWindow="-3140" windowWidth="20340" windowHeight="20140" xr2:uid="{7EA8B866-5E4B-4CBD-B814-F254738EF465}"/>
   </bookViews>
   <sheets>
     <sheet name="pIRfusiX_sensorBoard_BOM" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="157">
   <si>
     <t>Comment</t>
   </si>
@@ -487,16 +487,49 @@
   </si>
   <si>
     <t>used this instead: ‎ERA-3ARW122V‎</t>
+  </si>
+  <si>
+    <t>Here</t>
+  </si>
+  <si>
+    <t>hERE</t>
+  </si>
+  <si>
+    <t>HERE</t>
+  </si>
+  <si>
+    <t>MISSING</t>
+  </si>
+  <si>
+    <t>here</t>
+  </si>
+  <si>
+    <t>0.01uF</t>
+  </si>
+  <si>
+    <t>X used C0603C103K3RAC7867</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -563,7 +596,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -581,6 +614,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -898,18 +934,18 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="6" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -929,7 +965,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="80" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -951,8 +987,11 @@
       <c r="G2" s="5" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H2" s="8" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -974,8 +1013,11 @@
       <c r="G3" s="5" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="H3" s="8" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="96" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
@@ -997,8 +1039,11 @@
       <c r="G4" s="5" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H4" s="8" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>21</v>
       </c>
@@ -1020,8 +1065,11 @@
       <c r="G5" s="6" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="H5" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>25</v>
       </c>
@@ -1043,12 +1091,17 @@
       <c r="G6" s="6" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H6" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="4"/>
+      <c r="B7" s="4" t="s">
+        <v>155</v>
+      </c>
       <c r="C7" s="3" t="s">
         <v>31</v>
       </c>
@@ -1062,10 +1115,13 @@
         <v>1</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="80" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>33</v>
       </c>
@@ -1087,8 +1143,11 @@
       <c r="G8" s="6" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="H8" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>38</v>
       </c>
@@ -1110,8 +1169,11 @@
       <c r="G9" s="6" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H9" s="7" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>43</v>
       </c>
@@ -1133,8 +1195,11 @@
       <c r="G10" s="6" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H10" s="7" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>48</v>
       </c>
@@ -1156,8 +1221,11 @@
       <c r="G11" s="6" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H11" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>53</v>
       </c>
@@ -1179,8 +1247,11 @@
       <c r="G12" s="6" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H12" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>58</v>
       </c>
@@ -1200,8 +1271,11 @@
       <c r="G13" s="6" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H13" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>60</v>
       </c>
@@ -1223,8 +1297,11 @@
       <c r="G14" s="6" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="H14" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>65</v>
       </c>
@@ -1246,8 +1323,11 @@
       <c r="G15" s="6" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="H15" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>70</v>
       </c>
@@ -1269,8 +1349,11 @@
       <c r="G16" s="6" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="H16" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>75</v>
       </c>
@@ -1292,8 +1375,11 @@
       <c r="G17" s="6" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H17" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>80</v>
       </c>
@@ -1313,8 +1399,11 @@
       <c r="G18" s="6" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="H18" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="96" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>83</v>
       </c>
@@ -1336,8 +1425,11 @@
       <c r="G19" s="6" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="H19" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>88</v>
       </c>
@@ -1356,8 +1448,11 @@
       <c r="F20" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="H20" s="8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="80" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>93</v>
       </c>
@@ -1377,8 +1472,11 @@
       <c r="G21" s="6" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="H21" s="8" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="80" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>97</v>
       </c>
@@ -1400,8 +1498,11 @@
       <c r="G22" s="6" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="H22" s="7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>101</v>
       </c>
@@ -1423,8 +1524,11 @@
       <c r="G23" s="6" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="H23" s="7" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="80" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>106</v>
       </c>
@@ -1446,8 +1550,11 @@
       <c r="G24" s="6" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H24" s="7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>111</v>
       </c>
@@ -1469,8 +1576,11 @@
       <c r="G25" s="6" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H25" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>116</v>
       </c>
@@ -1489,8 +1599,11 @@
       <c r="F26" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="H26" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>121</v>
       </c>
@@ -1509,8 +1622,11 @@
       <c r="F27" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H27" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>125</v>
       </c>
@@ -1529,8 +1645,11 @@
       <c r="F28" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="H28" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="80" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>130</v>
       </c>
@@ -1549,8 +1668,11 @@
       <c r="F29" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="H29" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="96" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>134</v>
       </c>
@@ -1570,7 +1692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>138</v>
       </c>

</xml_diff>